<commit_message>
fixed bug in output bias calculation
</commit_message>
<xml_diff>
--- a/evaluation/top3results.xlsx
+++ b/evaluation/top3results.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="28060" windowHeight="15940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="46">
   <si>
     <t>rank</t>
   </si>
@@ -140,13 +145,25 @@
   </si>
   <si>
     <t>MedicareForAll</t>
+  </si>
+  <si>
+    <t>average top 3</t>
+  </si>
+  <si>
+    <t>OB Rank 3</t>
+  </si>
+  <si>
+    <t>53.3?</t>
+  </si>
+  <si>
+    <t>73.3?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,15 +180,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -194,15 +217,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,14 +547,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,8 +569,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -525,7 +587,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -536,7 +598,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -546,8 +608,16 @@
       <c r="C4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <f>SUM(C2:C4)/3</f>
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <f>(C2+AVERAGE(C2:C3) + AVERAGE(C2:C4))/3</f>
+        <v>76.666666666666671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1</v>
       </c>
@@ -558,7 +628,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2</v>
       </c>
@@ -569,7 +639,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>3</v>
       </c>
@@ -579,8 +649,16 @@
       <c r="C7">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <f>SUM(C5:C7)/3</f>
+        <v>80</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F5:F21" si="0">(C5+AVERAGE(C5:C6) + AVERAGE(C5:C7))/3</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>1</v>
       </c>
@@ -591,7 +669,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2</v>
       </c>
@@ -602,7 +680,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>3</v>
       </c>
@@ -612,8 +690,16 @@
       <c r="C10">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <f>SUM(C8:C10)/3</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>64.444444444444443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1</v>
       </c>
@@ -624,7 +710,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>2</v>
       </c>
@@ -635,7 +721,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>3</v>
       </c>
@@ -645,8 +731,16 @@
       <c r="C13">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <f>SUM(C11:C13)/3</f>
+        <v>80</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>1</v>
       </c>
@@ -657,7 +751,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>2</v>
       </c>
@@ -668,7 +762,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>3</v>
       </c>
@@ -678,8 +772,16 @@
       <c r="C16">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <f>SUM(C14:C16)/3</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>61.111111111111107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>1</v>
       </c>
@@ -690,7 +792,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>2</v>
       </c>
@@ -701,7 +803,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>3</v>
       </c>
@@ -711,8 +813,16 @@
       <c r="C19">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <f>SUM(C17:C19)/3</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>75.555555555555557</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>1</v>
       </c>
@@ -723,7 +833,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>3</v>
       </c>
@@ -733,8 +843,16 @@
       <c r="C21">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <f>SUM(C20:C21)/2</f>
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <f>(C20+AVERAGE(C20:C21))/2</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>1</v>
       </c>
@@ -745,7 +863,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>2</v>
       </c>
@@ -756,7 +874,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>3</v>
       </c>
@@ -766,8 +884,16 @@
       <c r="C24">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <f>SUM(C22:C24)/3</f>
+        <v>40</v>
+      </c>
+      <c r="F24">
+        <f>(C22+AVERAGE(C22:C23) + AVERAGE(C22:C24))/3</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>1</v>
       </c>
@@ -778,7 +904,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>2</v>
       </c>
@@ -789,7 +915,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>3</v>
       </c>
@@ -799,8 +925,16 @@
       <c r="C27">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27">
+        <f>SUM(C25:C27)/3</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F25:F88" si="1">(C25+AVERAGE(C25:C26) + AVERAGE(C25:C27))/3</f>
+        <v>44.44444444444445</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>1</v>
       </c>
@@ -810,8 +944,12 @@
       <c r="C28">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="H28">
+        <f>(80+((80+40)/2))/2</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>3</v>
       </c>
@@ -821,8 +959,19 @@
       <c r="C29">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29">
+        <f>SUM(C28:C29)/2</f>
+        <v>60</v>
+      </c>
+      <c r="F29" s="4">
+        <f>(C28+AVERAGE(C28:C29))/2</f>
+        <v>70</v>
+      </c>
+      <c r="G29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>1</v>
       </c>
@@ -833,7 +982,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>2</v>
       </c>
@@ -844,7 +993,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>3</v>
       </c>
@@ -854,8 +1003,16 @@
       <c r="C32">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32">
+        <f>SUM(C30:C32)/3</f>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>85.555555555555557</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>1</v>
       </c>
@@ -866,7 +1023,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>2</v>
       </c>
@@ -877,7 +1034,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>3</v>
       </c>
@@ -887,8 +1044,16 @@
       <c r="C35">
         <v>80</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35">
+        <f>SUM(C33:C35)/3</f>
+        <v>80</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>1</v>
       </c>
@@ -899,7 +1064,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>2</v>
       </c>
@@ -910,7 +1075,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>3</v>
       </c>
@@ -920,8 +1085,16 @@
       <c r="C38">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38">
+        <f>SUM(C36:C38)/3</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>68.8888888888889</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>2</v>
       </c>
@@ -932,7 +1105,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>3</v>
       </c>
@@ -942,8 +1115,16 @@
       <c r="C40">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40">
+        <f>SUM(C39:C40)/2</f>
+        <v>80</v>
+      </c>
+      <c r="F40">
+        <f>(C39+AVERAGE(C39:C40))/2</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>1</v>
       </c>
@@ -954,7 +1135,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>2</v>
       </c>
@@ -965,7 +1146,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>3</v>
       </c>
@@ -975,8 +1156,16 @@
       <c r="C43">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43">
+        <f>SUM(C41:C43)/3</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>64.444444444444443</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>2</v>
       </c>
@@ -986,8 +1175,14 @@
       <c r="C44">
         <v>80</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44">
+        <v>80</v>
+      </c>
+      <c r="F44">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>1</v>
       </c>
@@ -998,7 +1193,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1009,7 +1204,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>3</v>
       </c>
@@ -1019,8 +1214,16 @@
       <c r="C47">
         <v>40</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47">
+        <f>SUM(C45:C47)/3</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>51.111111111111114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>1</v>
       </c>
@@ -1031,7 +1234,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1042,7 +1245,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1052,8 +1255,16 @@
       <c r="C50">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50">
+        <f>SUM(C48:C50)/3</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>64.444444444444443</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>1</v>
       </c>
@@ -1064,7 +1275,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>2</v>
       </c>
@@ -1075,7 +1286,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>3</v>
       </c>
@@ -1085,8 +1296,16 @@
       <c r="C53">
         <v>100</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53">
+        <f>SUM(C51:C53)/3</f>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>87.777777777777771</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>1</v>
       </c>
@@ -1097,7 +1316,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>2</v>
       </c>
@@ -1108,7 +1327,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>3</v>
       </c>
@@ -1118,8 +1337,16 @@
       <c r="C56">
         <v>40</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56">
+        <f>SUM(C54:C56)/3</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>51.111111111111114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>1</v>
       </c>
@@ -1130,7 +1357,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1141,7 +1368,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>3</v>
       </c>
@@ -1151,8 +1378,16 @@
       <c r="C59">
         <v>100</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59">
+        <f>SUM(C57:C59)/3</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>57.777777777777771</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1163,7 +1398,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>2</v>
       </c>
@@ -1174,7 +1409,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>3</v>
       </c>
@@ -1184,8 +1419,16 @@
       <c r="C62">
         <v>80</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62">
+        <f>SUM(C60:C62)/3</f>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>92.222222222222229</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>1</v>
       </c>
@@ -1196,7 +1439,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>2</v>
       </c>
@@ -1207,7 +1450,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:6">
       <c r="A65">
         <v>3</v>
       </c>
@@ -1217,8 +1460,16 @@
       <c r="C65">
         <v>100</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="D65">
+        <f>SUM(C63:C65)/3</f>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>82.222222222222229</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66">
         <v>1</v>
       </c>
@@ -1229,7 +1480,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:6">
       <c r="A67">
         <v>2</v>
       </c>
@@ -1240,7 +1491,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:6">
       <c r="A68">
         <v>3</v>
       </c>
@@ -1250,8 +1501,16 @@
       <c r="C68">
         <v>40</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68">
+        <f>SUM(C66:C68)/3</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>81.1111111111111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69">
         <v>1</v>
       </c>
@@ -1262,7 +1521,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:6">
       <c r="A70">
         <v>2</v>
       </c>
@@ -1273,7 +1532,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:6">
       <c r="A71">
         <v>3</v>
       </c>
@@ -1283,8 +1542,16 @@
       <c r="C71">
         <v>80</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="D71">
+        <f>SUM(C69:C71)/3</f>
+        <v>80</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72">
         <v>1</v>
       </c>
@@ -1295,7 +1562,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:6">
       <c r="A73">
         <v>3</v>
       </c>
@@ -1305,8 +1572,16 @@
       <c r="C73">
         <v>80</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73">
+        <f>SUM(C72:C73)/2</f>
+        <v>80</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74">
         <v>1</v>
       </c>
@@ -1317,7 +1592,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:6">
       <c r="A75">
         <v>2</v>
       </c>
@@ -1328,7 +1603,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:6">
       <c r="A76">
         <v>3</v>
       </c>
@@ -1338,8 +1613,16 @@
       <c r="C76">
         <v>100</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76">
+        <f>SUM(C74:C76)/3</f>
+        <v>80</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>63.333333333333336</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77">
         <v>1</v>
       </c>
@@ -1350,7 +1633,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:6">
       <c r="A78">
         <v>2</v>
       </c>
@@ -1361,7 +1644,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:6">
       <c r="A79">
         <v>3</v>
       </c>
@@ -1371,8 +1654,16 @@
       <c r="C79">
         <v>100</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="D79">
+        <f>SUM(C77:C79)/3</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>57.777777777777771</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80">
         <v>1</v>
       </c>
@@ -1383,7 +1674,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:8">
       <c r="A81">
         <v>2</v>
       </c>
@@ -1394,7 +1685,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:8">
       <c r="A82">
         <v>3</v>
       </c>
@@ -1404,8 +1695,16 @@
       <c r="C82">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="D82">
+        <f>SUM(C80:C82)/3</f>
+        <v>80</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83">
         <v>2</v>
       </c>
@@ -1416,7 +1715,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:8">
       <c r="A84">
         <v>3</v>
       </c>
@@ -1426,8 +1725,16 @@
       <c r="C84">
         <v>80</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="D84">
+        <f>SUM(C83:C84)/2</f>
+        <v>80</v>
+      </c>
+      <c r="F84" s="5">
+        <f>(C83+AVERAGE(C83:C84))/2</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85">
         <v>2</v>
       </c>
@@ -1438,7 +1745,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:8">
       <c r="A86">
         <v>3</v>
       </c>
@@ -1448,8 +1755,16 @@
       <c r="C86">
         <v>40</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="D86">
+        <f>SUM(C85:C86)/2</f>
+        <v>60</v>
+      </c>
+      <c r="F86" s="5">
+        <f>(C85+AVERAGE(C85:C86))/2</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87">
         <v>1</v>
       </c>
@@ -1460,7 +1775,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:8">
       <c r="A88">
         <v>2</v>
       </c>
@@ -1471,7 +1786,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:8">
       <c r="A89">
         <v>3</v>
       </c>
@@ -1481,8 +1796,16 @@
       <c r="C89">
         <v>80</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="D89">
+        <f>SUM(C87:C89)/3</f>
+        <v>80</v>
+      </c>
+      <c r="F89">
+        <f t="shared" ref="F89:F109" si="2">(C87+AVERAGE(C87:C88) + AVERAGE(C87:C89))/3</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90">
         <v>1</v>
       </c>
@@ -1493,7 +1816,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:8">
       <c r="A91">
         <v>2</v>
       </c>
@@ -1504,7 +1827,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:8">
       <c r="A92">
         <v>3</v>
       </c>
@@ -1514,8 +1837,16 @@
       <c r="C92">
         <v>100</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="D92">
+        <f>SUM(C90:C92)/3</f>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="2"/>
+        <v>71.1111111111111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93">
         <v>1</v>
       </c>
@@ -1526,7 +1857,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:8">
       <c r="A94">
         <v>2</v>
       </c>
@@ -1536,8 +1867,23 @@
       <c r="C94">
         <v>80</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="D94">
+        <f>SUM(C93:C94)/2</f>
+        <v>60</v>
+      </c>
+      <c r="F94" s="4">
+        <f>(C93+AVERAGE(C93:C94))/2</f>
+        <v>50</v>
+      </c>
+      <c r="G94" t="s">
+        <v>44</v>
+      </c>
+      <c r="H94">
+        <f>(40 + ((40+80)/2) +((40+80)/2))/3</f>
+        <v>53.333333333333336</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95">
         <v>1</v>
       </c>
@@ -1548,7 +1894,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:8">
       <c r="A96">
         <v>2</v>
       </c>
@@ -1559,7 +1905,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:6">
       <c r="A97">
         <v>3</v>
       </c>
@@ -1569,8 +1915,16 @@
       <c r="C97">
         <v>40</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="D97">
+        <f>SUM(C95:C97)/3</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="2"/>
+        <v>64.444444444444443</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98">
         <v>1</v>
       </c>
@@ -1581,7 +1935,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:6">
       <c r="A99">
         <v>2</v>
       </c>
@@ -1592,7 +1946,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:6">
       <c r="A100">
         <v>3</v>
       </c>
@@ -1602,8 +1956,16 @@
       <c r="C100">
         <v>80</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="D100">
+        <f>SUM(C98:C100)/3</f>
+        <v>80</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101">
         <v>1</v>
       </c>
@@ -1614,7 +1976,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:6">
       <c r="A102">
         <v>2</v>
       </c>
@@ -1625,7 +1987,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:6">
       <c r="A103">
         <v>3</v>
       </c>
@@ -1635,8 +1997,16 @@
       <c r="C103">
         <v>80</v>
       </c>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="D103">
+        <f>SUM(C101:C103)/3</f>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="2"/>
+        <v>85.555555555555557</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104">
         <v>1</v>
       </c>
@@ -1647,7 +2017,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:6">
       <c r="A105">
         <v>2</v>
       </c>
@@ -1658,7 +2028,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:6">
       <c r="A106">
         <v>3</v>
       </c>
@@ -1668,8 +2038,16 @@
       <c r="C106">
         <v>80</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="D106">
+        <f>SUM(C104:C106)/3</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="2"/>
+        <v>44.44444444444445</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107">
         <v>1</v>
       </c>
@@ -1680,7 +2058,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:6">
       <c r="A108">
         <v>2</v>
       </c>
@@ -1691,7 +2069,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:6">
       <c r="A109">
         <v>3</v>
       </c>
@@ -1701,8 +2079,45 @@
       <c r="C109">
         <v>40</v>
       </c>
+      <c r="D109">
+        <f>SUM(C107:C109)/3</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="2"/>
+        <v>51.111111111111114</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="D110">
+        <f>AVERAGE(D2:D109)</f>
+        <v>70.256410256410263</v>
+      </c>
+      <c r="F110">
+        <f>AVERAGE(F2:F109)</f>
+        <v>70.170940170940185</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="D111">
+        <f>COUNT(D2:D109)</f>
+        <v>39</v>
+      </c>
+      <c r="E111">
+        <f t="shared" ref="E111:F111" si="3">COUNT(E2:E109)</f>
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>